<commit_message>
add filereader to enable file uploads
</commit_message>
<xml_diff>
--- a/VoorbeeldCv.xlsx
+++ b/VoorbeeldCv.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\CvViewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{614FF318-8B98-4706-9CFA-4B5F222BE15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92B665C4-5D9C-486A-BE0C-DC2F82FC053E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65172" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="6" xr2:uid="{8D48BAE9-DB51-4951-9C96-C25F693C6267}"/>
+    <workbookView xWindow="34452" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="675" xr2:uid="{8D48BAE9-DB51-4951-9C96-C25F693C6267}"/>
   </bookViews>
   <sheets>
-    <sheet name="Adres" sheetId="2" r:id="rId1"/>
-    <sheet name="Auteur" sheetId="1" r:id="rId2"/>
-    <sheet name="Contactgegevens" sheetId="4" r:id="rId3"/>
-    <sheet name="Certificaten" sheetId="3" r:id="rId4"/>
-    <sheet name="Opleidingen" sheetId="5" r:id="rId5"/>
-    <sheet name="Vaardigheden" sheetId="6" r:id="rId6"/>
-    <sheet name="Werkervaring" sheetId="7" r:id="rId7"/>
+    <sheet name="Meta" sheetId="8" r:id="rId1"/>
+    <sheet name="Adres" sheetId="2" r:id="rId2"/>
+    <sheet name="Auteur" sheetId="1" r:id="rId3"/>
+    <sheet name="Contactgegevens" sheetId="4" r:id="rId4"/>
+    <sheet name="Certificaten" sheetId="3" r:id="rId5"/>
+    <sheet name="Opleidingen" sheetId="5" r:id="rId6"/>
+    <sheet name="Vaardigheden" sheetId="6" r:id="rId7"/>
+    <sheet name="Werkervaring" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
   <si>
     <t>Voornaam</t>
   </si>
@@ -252,6 +253,12 @@
   </si>
   <si>
     <t>Vertalen van (Brits) Engels naar Nederlands (en soms andersom). Copywriting en algemene werkzaamheden opgepakt binnen het marketingteam.</t>
+  </si>
+  <si>
+    <t>Inleiding</t>
+  </si>
+  <si>
+    <t>Gemotiveerde en technisch georiënteerde IT-professional met oog voor detail. Via een éénjarig traineeship klaargestoomd voor een carrière als .NET-developer. Gestart bij afdeling Toeslagen en snel doorgegroeid naar medior niveau. Mijn kwaliteiten liggen in het identificeren en doorgronden van problemen, mijn leergierigheid en mijn vermogen om zelfstandig te kunnen werken, maar ook afstemming te zoeken waar dat nodig is.</t>
   </si>
 </sst>
 </file>
@@ -639,11 +646,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1F48E1-6AC7-43BF-B2D8-433EBAF7D67B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F650FE90-CE88-45A5-8823-32926307413D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -694,7 +726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D16574-FF57-424C-B8CF-3C19683AAF42}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -731,7 +763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF1090E-301B-4882-A4AF-C0BBE1FDEB5D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -775,12 +807,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E0FFEA-5BE9-4D31-87BD-541A6DC76292}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -881,12 +913,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F2CD81-A709-4D71-9128-FDE71ADCE9EE}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -979,7 +1011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0CA33D-BF5F-4756-A867-964545418DA6}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1050,11 +1082,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B87A408-4E02-4894-91A0-8C31F217AA82}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>